<commit_message>
Auto stash before merge of "master" and "Robert-Sheehy/master"
</commit_message>
<xml_diff>
--- a/Project Documents/Penguin Description.xlsx
+++ b/Project Documents/Penguin Description.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00139303\Documents\Push-Penguin-3D\Documents\Revised Excel sheet\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Template for Items (2)" sheetId="5" r:id="rId1"/>
@@ -17,13 +12,14 @@
     <sheet name="Penguin" sheetId="2" r:id="rId3"/>
     <sheet name="Enemies" sheetId="3" r:id="rId4"/>
     <sheet name="Template for Items" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
   <si>
     <t>Characters</t>
   </si>
@@ -122,16 +118,96 @@
   </si>
   <si>
     <t>David O'Sullivan - penguins</t>
+  </si>
+  <si>
+    <t>Main Player -Interacts with all Phsical objects in game.</t>
+  </si>
+  <si>
+    <t>Can turn 360 degres</t>
+  </si>
+  <si>
+    <t>Player and camera can look all around the scene</t>
+  </si>
+  <si>
+    <t>Can move 360 degrees</t>
+  </si>
+  <si>
+    <t>Player can move 360 degrees through a combination of directional controls</t>
+  </si>
+  <si>
+    <t>Can Push</t>
+  </si>
+  <si>
+    <t>Player can activate/interact with a certain object(s) to make that object accelerate in a desired direction</t>
+  </si>
+  <si>
+    <t>Collision</t>
+  </si>
+  <si>
+    <t>Ice Block</t>
+  </si>
+  <si>
+    <t>Can Destroy</t>
+  </si>
+  <si>
+    <t>Player can activate/interact with an object to destroy it</t>
+  </si>
+  <si>
+    <t>Pick-up Items, Ice Block</t>
+  </si>
+  <si>
+    <t>Can be restrained in movement</t>
+  </si>
+  <si>
+    <t>Player can be interrupted during movement when certain objects impede the player</t>
+  </si>
+  <si>
+    <t>Stop Moving</t>
+  </si>
+  <si>
+    <t>Enemies, World, Ice Block, Rock</t>
+  </si>
+  <si>
+    <t>Can be damaged/destroyed</t>
+  </si>
+  <si>
+    <t>Player can be hurt/killed causing a loss of previously accumulated points or death</t>
+  </si>
+  <si>
+    <t>Enemies, World.</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Player is spawned on to the map by the world</t>
+  </si>
+  <si>
+    <t>(-)H.P. or Death</t>
+  </si>
+  <si>
+    <t>Poosition</t>
+  </si>
+  <si>
+    <t>Damageable, Killable, Movement, Spawnable, CanPush, CanLook, CanDestroy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -154,13 +230,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -219,7 +298,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -254,7 +333,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -463,16 +542,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="92.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -493,7 +572,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -506,7 +585,18 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -525,7 +615,30 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -544,15 +657,52 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>30</v>
       </c>
-      <c r="B17" t="s">
-        <v>31</v>
+      <c r="B19" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -565,7 +715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -778,4 +928,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>